<commit_message>
1) Modified the format of the 'Meta' sheet in the result file output by '_write_selected_variables_to_excel' to improve the readability.
2) Modified the 'Kearsley_GSP_group_only_modified.xlsx' so that currently all demands have power factor = 1, therefore no reactive loads.

3) According to 2), the power balance and power flow constraints in 'build_investment_model' and 'build_normal_scenario_opf_model' investment_model.py are modified.
</commit_message>
<xml_diff>
--- a/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only_modified.xlsx
+++ b/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only_modified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\Manchester_Distribution_Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03159D6F-073C-4AFD-BB90-F6314FEFC9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B84A32-21BD-497D-918C-E8EF0B9854F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_values" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="146">
   <si>
     <t>Name</t>
   </si>
@@ -467,6 +467,15 @@
   </si>
   <si>
     <t>all impedance values (R and X) at both tn and dn levels are multiplied by a factor 0.1</t>
+  </si>
+  <si>
+    <t>Scale_Factor</t>
+  </si>
+  <si>
+    <t>Sd_max_original</t>
+  </si>
+  <si>
+    <t>Sd_min_original</t>
   </si>
 </sst>
 </file>
@@ -852,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:L2"/>
+    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3459,7 +3468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
@@ -7011,10 +7020,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7023,10 +7032,13 @@
     <col min="3" max="3" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.59765625" customWidth="1"/>
     <col min="6" max="6" width="12.06640625" customWidth="1"/>
-    <col min="7" max="10" width="10.59765625" customWidth="1"/>
+    <col min="7" max="11" width="10.59765625" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -7057,8 +7069,17 @@
       <c r="J1" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="L1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>10</v>
       </c>
@@ -7069,32 +7090,42 @@
         <v>27</v>
       </c>
       <c r="D2">
-        <v>62.990131895094009</v>
+        <f>L2*N2</f>
+        <v>56.6911187055846</v>
       </c>
       <c r="E2">
         <v>15.17744077</v>
       </c>
       <c r="F2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G28" si="0">D2*F2</f>
-        <v>59.840625300339305</v>
+        <v>56.6911187055846</v>
       </c>
       <c r="H2">
         <f t="shared" ref="H2:H28" si="1">E2*F2</f>
-        <v>14.418568731500001</v>
+        <v>15.17744077</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I28" si="2">D2*SQRT(1-F2^2)</f>
-        <v>19.668662380185662</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <f t="shared" ref="J2:J28" si="3">E2*SQRT(1-F2^2)</f>
-        <v>4.7391543614730134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>62.990131895094002</v>
+      </c>
+      <c r="M2">
+        <v>15.17744077</v>
+      </c>
+      <c r="N2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>11</v>
       </c>
@@ -7105,32 +7136,42 @@
         <v>34</v>
       </c>
       <c r="D3">
-        <v>80.871689211959065</v>
+        <f t="shared" ref="D3:D28" si="4">L3*N3</f>
+        <v>72.784520290763155</v>
       </c>
       <c r="E3">
         <v>29.73106675</v>
       </c>
       <c r="F3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>76.82810475136111</v>
+        <v>72.784520290763155</v>
       </c>
       <c r="H3">
         <f t="shared" si="1"/>
-        <v>28.244513412499998</v>
+        <v>29.73106675</v>
       </c>
       <c r="I3">
         <f t="shared" si="2"/>
-        <v>25.252176862789089</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <f t="shared" si="3"/>
-        <v>9.2835226171999601</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>80.871689211959065</v>
+      </c>
+      <c r="M3">
+        <v>29.73106675</v>
+      </c>
+      <c r="N3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>12</v>
       </c>
@@ -7141,32 +7182,42 @@
         <v>42</v>
       </c>
       <c r="D4">
-        <v>100.87403825175321</v>
+        <f t="shared" si="4"/>
+        <v>90.786634426577891</v>
       </c>
       <c r="E4">
         <v>28.2818364</v>
       </c>
       <c r="F4">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>95.830336339165541</v>
+        <v>90.786634426577891</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>26.867744579999997</v>
+        <v>28.2818364</v>
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
-        <v>31.497908348628119</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <f t="shared" si="3"/>
-        <v>8.8310005854515499</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>100.87403825175321</v>
+      </c>
+      <c r="M4">
+        <v>28.2818364</v>
+      </c>
+      <c r="N4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>13</v>
       </c>
@@ -7177,32 +7228,42 @@
         <v>55</v>
       </c>
       <c r="D5">
-        <v>70.824781345557497</v>
+        <f t="shared" si="4"/>
+        <v>63.742303211001747</v>
       </c>
       <c r="E5">
         <v>16.48118156</v>
       </c>
       <c r="F5">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>67.283542278279626</v>
+        <v>63.742303211001747</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>15.657122481999998</v>
+        <v>16.48118156</v>
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>22.115030887000543</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <f t="shared" si="3"/>
-        <v>5.1462472926720304</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>70.824781345557497</v>
+      </c>
+      <c r="M5">
+        <v>16.48118156</v>
+      </c>
+      <c r="N5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>46</v>
       </c>
@@ -7213,32 +7274,43 @@
         <v>104</v>
       </c>
       <c r="D6">
-        <v>15.817738160351359</v>
+        <f t="shared" si="4"/>
+        <v>9.73596434431626</v>
       </c>
       <c r="E6">
         <v>3.9445701560000002</v>
       </c>
       <c r="F6">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>15.02685125233379</v>
+        <v>9.73596434431626</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>3.7473416481999999</v>
+        <v>3.9445701560000002</v>
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>4.9390871575292108</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <f t="shared" si="3"/>
-        <v>1.2316916364381032</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f>15.8177381603514-5</f>
+        <v>10.8177381603514</v>
+      </c>
+      <c r="M6">
+        <v>3.9445701560000002</v>
+      </c>
+      <c r="N6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>47</v>
       </c>
@@ -7249,32 +7321,42 @@
         <v>105</v>
       </c>
       <c r="D7">
-        <v>8.7183809790987699</v>
+        <f t="shared" si="4"/>
+        <v>7.8465428811888929</v>
       </c>
       <c r="E7">
         <v>2.2605684429999999</v>
       </c>
       <c r="F7">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>8.2824619301438318</v>
+        <v>7.8465428811888929</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>2.1475400208499997</v>
+        <v>2.2605684429999999</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>2.7223135881873248</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <f t="shared" si="3"/>
-        <v>0.70586227008887925</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>8.7183809790987699</v>
+      </c>
+      <c r="M7">
+        <v>2.2605684429999999</v>
+      </c>
+      <c r="N7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>48</v>
       </c>
@@ -7285,32 +7367,42 @@
         <v>106</v>
       </c>
       <c r="D8">
-        <v>14.745301948651541</v>
+        <f t="shared" si="4"/>
+        <v>13.270771753786388</v>
       </c>
       <c r="E8">
         <v>4.0282644999999997</v>
       </c>
       <c r="F8">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>14.008036851218963</v>
+        <v>13.270771753786388</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>3.8268512749999997</v>
+        <v>4.0282644999999997</v>
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>4.6042190577554445</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <f t="shared" si="3"/>
-        <v>1.2578251869759665</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>14.745301948651541</v>
+      </c>
+      <c r="M8">
+        <v>4.0282644999999997</v>
+      </c>
+      <c r="N8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>49</v>
       </c>
@@ -7321,32 +7413,42 @@
         <v>107</v>
       </c>
       <c r="D9">
-        <v>9.3392216532809886</v>
+        <f t="shared" si="4"/>
+        <v>8.4052994879528899</v>
       </c>
       <c r="E9">
         <v>2.7367567159999999</v>
       </c>
       <c r="F9">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>8.8722605706169393</v>
+        <v>8.4052994879528899</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>2.5999188801999997</v>
+        <v>2.7367567159999999</v>
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>2.9161710265669383</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <f t="shared" si="3"/>
-        <v>0.85455201067616882</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>9.3392216532809886</v>
+      </c>
+      <c r="M9">
+        <v>2.7367567159999999</v>
+      </c>
+      <c r="N9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>50</v>
       </c>
@@ -7357,32 +7459,42 @@
         <v>108</v>
       </c>
       <c r="D10">
-        <v>10.66381232746668</v>
+        <f t="shared" si="4"/>
+        <v>9.5974310947200117</v>
       </c>
       <c r="E10">
         <v>2.8652334069999998</v>
       </c>
       <c r="F10">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>10.130621711093346</v>
+        <v>9.5974310947200117</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>2.7219717366499996</v>
+        <v>2.8652334069999998</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>3.3297743320162794</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <f t="shared" si="3"/>
-        <v>0.89466884458296125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>10.66381232746668</v>
+      </c>
+      <c r="M10">
+        <v>2.8652334069999998</v>
+      </c>
+      <c r="N10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>51</v>
       </c>
@@ -7393,32 +7505,42 @@
         <v>109</v>
       </c>
       <c r="D11">
-        <v>24.561448963248029</v>
+        <f t="shared" si="4"/>
+        <v>22.105304066923228</v>
       </c>
       <c r="E11">
         <v>6.0181003110000004</v>
       </c>
       <c r="F11">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>23.333376515085625</v>
+        <v>22.105304066923228</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>5.7171952954499998</v>
+        <v>6.0181003110000004</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>7.669309980662419</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <f t="shared" si="3"/>
-        <v>1.8791512198177893</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>24.561448963248029</v>
+      </c>
+      <c r="M11">
+        <v>6.0181003110000004</v>
+      </c>
+      <c r="N11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>52</v>
       </c>
@@ -7429,32 +7551,42 @@
         <v>110</v>
       </c>
       <c r="D12">
-        <v>17.18120772798412</v>
+        <f t="shared" si="4"/>
+        <v>15.463086955185709</v>
       </c>
       <c r="E12">
         <v>4.1625504160000002</v>
       </c>
       <c r="F12">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>16.322147341584913</v>
+        <v>15.463086955185709</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>3.9544228952</v>
+        <v>4.1625504160000002</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>5.3648303935663968</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <f t="shared" si="3"/>
-        <v>1.2997559508076213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>17.18120772798412</v>
+      </c>
+      <c r="M12">
+        <v>4.1625504160000002</v>
+      </c>
+      <c r="N12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>53</v>
       </c>
@@ -7465,32 +7597,42 @@
         <v>111</v>
       </c>
       <c r="D13">
-        <v>17.82439332308557</v>
+        <f t="shared" si="4"/>
+        <v>16.041953990777014</v>
       </c>
       <c r="E13">
         <v>5.440907954</v>
       </c>
       <c r="F13">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>16.933173656931292</v>
+        <v>16.041953990777014</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>5.1688625562999997</v>
+        <v>5.440907954</v>
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>5.565665031266759</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <f t="shared" si="3"/>
-        <v>1.6989229641099965</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>17.82439332308557</v>
+      </c>
+      <c r="M13">
+        <v>5.440907954</v>
+      </c>
+      <c r="N13">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>54</v>
       </c>
@@ -7501,32 +7643,42 @@
         <v>112</v>
       </c>
       <c r="D14">
-        <v>10.241879258445859</v>
+        <f t="shared" si="4"/>
+        <v>9.217691332601273</v>
       </c>
       <c r="E14">
         <v>2.4897486710000001</v>
       </c>
       <c r="F14">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>9.7297852955235662</v>
+        <v>9.217691332601273</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>2.3652612374499999</v>
+        <v>2.4897486710000001</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>3.1980257734416235</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <f t="shared" si="3"/>
-        <v>0.77742377334550383</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>10.241879258445859</v>
+      </c>
+      <c r="M14">
+        <v>2.4897486710000001</v>
+      </c>
+      <c r="N14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>55</v>
       </c>
@@ -7537,32 +7689,42 @@
         <v>113</v>
       </c>
       <c r="D15">
-        <v>6.0517216763918684</v>
+        <f t="shared" si="4"/>
+        <v>5.4465495087526818</v>
       </c>
       <c r="E15">
         <v>1.1628632670000001</v>
       </c>
       <c r="F15">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>5.7491355925722747</v>
+        <v>5.4465495087526818</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
-        <v>1.1047201036500001</v>
+        <v>1.1628632670000001</v>
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>1.8896494877965713</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <f t="shared" si="3"/>
-        <v>0.3631039387413012</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>6.0517216763918684</v>
+      </c>
+      <c r="M15">
+        <v>1.1628632670000001</v>
+      </c>
+      <c r="N15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>56</v>
       </c>
@@ -7573,32 +7735,43 @@
         <v>114</v>
       </c>
       <c r="D16">
-        <v>12.48369329419058</v>
+        <f t="shared" si="4"/>
+        <v>8.5353239647715391</v>
       </c>
       <c r="E16">
         <v>3.3592794110000002</v>
       </c>
       <c r="F16">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>11.85950862948105</v>
+        <v>8.5353239647715391</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
-        <v>3.1913154404499999</v>
+        <v>3.3592794110000002</v>
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>3.8980319817419846</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <f t="shared" si="3"/>
-        <v>1.0489346598877978</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>12.4836932941906-3</f>
+        <v>9.4836932941905996</v>
+      </c>
+      <c r="M16">
+        <v>3.3592794110000002</v>
+      </c>
+      <c r="N16">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>57</v>
       </c>
@@ -7609,32 +7782,42 @@
         <v>115</v>
       </c>
       <c r="D17">
-        <v>9.2036618442419424</v>
+        <f t="shared" si="4"/>
+        <v>8.2832956598177478</v>
       </c>
       <c r="E17">
         <v>2.478126638</v>
       </c>
       <c r="F17">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>8.7434787520298443</v>
+        <v>8.2832956598177478</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
-        <v>2.3542203060999998</v>
+        <v>2.478126638</v>
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>2.8738424897613326</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <f t="shared" si="3"/>
-        <v>0.77379479470438772</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>9.2036618442419424</v>
+      </c>
+      <c r="M17">
+        <v>2.478126638</v>
+      </c>
+      <c r="N17">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>58</v>
       </c>
@@ -7645,32 +7828,42 @@
         <v>116</v>
       </c>
       <c r="D18">
-        <v>11.25342699086633</v>
+        <f t="shared" si="4"/>
+        <v>10.128084291779698</v>
       </c>
       <c r="E18">
         <v>2.2924193000000002</v>
       </c>
       <c r="F18">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>10.690755641323014</v>
+        <v>10.128084291779698</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>2.1777983349999999</v>
+        <v>2.2924193000000002</v>
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>3.5138814516541377</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <f t="shared" si="3"/>
-        <v>0.71580769699949309</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>11.25342699086633</v>
+      </c>
+      <c r="M18">
+        <v>2.2924193000000002</v>
+      </c>
+      <c r="N18">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>59</v>
       </c>
@@ -7681,32 +7874,42 @@
         <v>117</v>
       </c>
       <c r="D19">
-        <v>13.51328567040467</v>
+        <f t="shared" si="4"/>
+        <v>12.161957103364204</v>
       </c>
       <c r="E19">
         <v>3.4044029509999998</v>
       </c>
       <c r="F19">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>12.837621386884436</v>
+        <v>12.161957103364204</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>3.2341828034499995</v>
+        <v>3.4044029509999998</v>
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>4.2195220981731465</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <f t="shared" si="3"/>
-        <v>1.0630244807368301</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>13.51328567040467</v>
+      </c>
+      <c r="M19">
+        <v>3.4044029509999998</v>
+      </c>
+      <c r="N19">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>60</v>
       </c>
@@ -7717,32 +7920,42 @@
         <v>118</v>
       </c>
       <c r="D20">
-        <v>12.471403817077681</v>
+        <f t="shared" si="4"/>
+        <v>11.224263435369913</v>
       </c>
       <c r="E20">
         <v>2.2515995869999998</v>
       </c>
       <c r="F20">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>11.847833626223796</v>
+        <v>11.224263435369913</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
-        <v>2.1390196076499999</v>
+        <v>2.2515995869999998</v>
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>3.8941945937434137</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <f t="shared" si="3"/>
-        <v>0.70306174570048308</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>12.471403817077681</v>
+      </c>
+      <c r="M20">
+        <v>2.2515995869999998</v>
+      </c>
+      <c r="N20">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>61</v>
       </c>
@@ -7753,32 +7966,42 @@
         <v>119</v>
       </c>
       <c r="D21">
-        <v>23.769442241105981</v>
+        <f t="shared" si="4"/>
+        <v>21.392498016995383</v>
       </c>
       <c r="E21">
         <v>6.1186455009999996</v>
       </c>
       <c r="F21">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>22.58097012905068</v>
+        <v>21.392498016995383</v>
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
-        <v>5.8127132259499996</v>
+        <v>6.1186455009999996</v>
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>7.4220059609376605</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
-        <v>1.9105464453327186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>23.769442241105981</v>
+      </c>
+      <c r="M21">
+        <v>6.1186455009999996</v>
+      </c>
+      <c r="N21">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>62</v>
       </c>
@@ -7789,32 +8012,42 @@
         <v>120</v>
       </c>
       <c r="D22">
-        <v>15.16358066810931</v>
+        <f t="shared" si="4"/>
+        <v>13.647222601298379</v>
       </c>
       <c r="E22">
         <v>3.6246869820000001</v>
       </c>
       <c r="F22">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>14.405401634703843</v>
+        <v>13.647222601298379</v>
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
-        <v>3.4434526328999997</v>
+        <v>3.6246869820000001</v>
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>4.7348265460447649</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
-        <v>1.1318081473705368</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>15.16358066810931</v>
+      </c>
+      <c r="M22">
+        <v>3.6246869820000001</v>
+      </c>
+      <c r="N22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>63</v>
       </c>
@@ -7825,32 +8058,42 @@
         <v>121</v>
       </c>
       <c r="D23">
-        <v>12.56492637502612</v>
+        <f t="shared" si="4"/>
+        <v>11.308433737523508</v>
       </c>
       <c r="E23">
         <v>3.190982521</v>
       </c>
       <c r="F23">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>11.936680056274813</v>
+        <v>11.308433737523508</v>
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
-        <v>3.0314333949500001</v>
+        <v>3.190982521</v>
       </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>3.9233970031030689</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <f t="shared" si="3"/>
-        <v>0.99638397282846392</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>12.56492637502612</v>
+      </c>
+      <c r="M23">
+        <v>3.190982521</v>
+      </c>
+      <c r="N23">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>64</v>
       </c>
@@ -7861,32 +8104,42 @@
         <v>122</v>
       </c>
       <c r="D24">
-        <v>12.583011408930631</v>
+        <f t="shared" si="4"/>
+        <v>11.324710268037569</v>
       </c>
       <c r="E24">
         <v>2.7713843219999998</v>
       </c>
       <c r="F24">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>11.953860838484099</v>
+        <v>11.324710268037569</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
-        <v>2.6328151058999998</v>
+        <v>2.7713843219999998</v>
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>3.9290440531298008</v>
+        <v>0</v>
       </c>
       <c r="J24">
         <f t="shared" si="3"/>
-        <v>0.86536447718413523</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>12.583011408930631</v>
+      </c>
+      <c r="M24">
+        <v>2.7713843219999998</v>
+      </c>
+      <c r="N24">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>65</v>
       </c>
@@ -7897,32 +8150,42 @@
         <v>123</v>
       </c>
       <c r="D25">
-        <v>10.343775674877429</v>
+        <f t="shared" si="4"/>
+        <v>9.3093981073896863</v>
       </c>
       <c r="E25">
         <v>2.5879858910000002</v>
       </c>
       <c r="F25">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>9.826586891133557</v>
+        <v>9.3093981073896863</v>
       </c>
       <c r="H25">
         <f t="shared" si="1"/>
-        <v>2.45858659645</v>
+        <v>2.5879858910000002</v>
       </c>
       <c r="I25">
         <f t="shared" si="2"/>
-        <v>3.2298429192745801</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <f t="shared" si="3"/>
-        <v>0.80809833545891496</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>10.343775674877429</v>
+      </c>
+      <c r="M25">
+        <v>2.5879858910000002</v>
+      </c>
+      <c r="N25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>66</v>
       </c>
@@ -7933,32 +8196,42 @@
         <v>124</v>
       </c>
       <c r="D26">
-        <v>9.1184429123599724</v>
+        <f t="shared" si="4"/>
+        <v>8.206598621123975</v>
       </c>
       <c r="E26">
         <v>2.5260950499999999</v>
       </c>
       <c r="F26">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>8.6625207667419737</v>
+        <v>8.206598621123975</v>
       </c>
       <c r="H26">
         <f t="shared" si="1"/>
-        <v>2.3997902974999996</v>
+        <v>2.5260950499999999</v>
       </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>2.8472328868099051</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <f t="shared" si="3"/>
-        <v>0.78877292655070519</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>9.1184429123599724</v>
+      </c>
+      <c r="M26">
+        <v>2.5260950499999999</v>
+      </c>
+      <c r="N26">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>67</v>
       </c>
@@ -7969,32 +8242,42 @@
         <v>125</v>
       </c>
       <c r="D27">
-        <v>12.03819464418018</v>
+        <f t="shared" si="4"/>
+        <v>10.834375179762162</v>
       </c>
       <c r="E27">
         <v>2.394727966</v>
       </c>
       <c r="F27">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>11.436284911971171</v>
+        <v>10.834375179762162</v>
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
-        <v>2.2749915676999999</v>
+        <v>2.394727966</v>
       </c>
       <c r="I27">
         <f t="shared" si="2"/>
-        <v>3.758925072861778</v>
+        <v>0</v>
       </c>
       <c r="J27">
         <f t="shared" si="3"/>
-        <v>0.74775356771893353</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>12.03819464418018</v>
+      </c>
+      <c r="M27">
+        <v>2.394727966</v>
+      </c>
+      <c r="N27">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>68</v>
       </c>
@@ -8005,29 +8288,39 @@
         <v>126</v>
       </c>
       <c r="D28">
-        <v>10.860025148287541</v>
+        <f t="shared" si="4"/>
+        <v>9.7740226334587863</v>
       </c>
       <c r="E28">
         <v>2.036662905</v>
       </c>
       <c r="F28">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>10.317023890873163</v>
+        <v>9.7740226334587863</v>
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
-        <v>1.9348297597499999</v>
+        <v>2.036662905</v>
       </c>
       <c r="I28">
         <f t="shared" si="2"/>
-        <v>3.3910417656805985</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <f t="shared" si="3"/>
-        <v>0.63594778825686349</v>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>10.860025148287541</v>
+      </c>
+      <c r="M28">
+        <v>2.036662905</v>
+      </c>
+      <c r="N28">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) In network_factory.py, updated the part 'elif name == Manchester_distribution_network_Kearsley' so that it can set different types of DGs based on the pre-defined renewable share for the DG at each DN bus.
2) The network.py is updated so that its initialisation includes setting the renewable generation profiles (scaled from a normalised profile for PV/wind) to each renewable DG at DN level.

3) The two-stage investment model investment_model_two_stage.py is updated to cope with the above-mentioned improvements. And it is updated to read the windstorm scenarios directly from the windstorm library generated by ws_scenario_library_generator.py.
</commit_message>
<xml_diff>
--- a/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only_modified.xlsx
+++ b/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only_modified.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\Manchester_Distribution_Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B84A32-21BD-497D-918C-E8EF0B9854F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ABD00E-65D7-41CD-82B1-E382242383E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_values" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="149">
   <si>
     <t>Name</t>
   </si>
@@ -476,6 +476,15 @@
   </si>
   <si>
     <t>Sd_min_original</t>
+  </si>
+  <si>
+    <t>Wind Share</t>
+  </si>
+  <si>
+    <t>PV Share</t>
+  </si>
+  <si>
+    <t>Gas Share</t>
   </si>
 </sst>
 </file>
@@ -861,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:D57"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3468,8 +3477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7022,7 +7031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -8330,10 +8339,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8343,9 +8352,11 @@
     <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="10.59765625" customWidth="1"/>
     <col min="9" max="10" width="15.59765625" customWidth="1"/>
+    <col min="11" max="11" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -8376,8 +8387,17 @@
       <c r="J1" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>10</v>
       </c>
@@ -8405,8 +8425,17 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>11</v>
       </c>
@@ -8434,8 +8463,17 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>12</v>
       </c>
@@ -8463,8 +8501,17 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>13</v>
       </c>
@@ -8492,8 +8539,17 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>46</v>
       </c>
@@ -8521,8 +8577,17 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>47</v>
       </c>
@@ -8550,8 +8615,17 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>48</v>
       </c>
@@ -8579,8 +8653,17 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>49</v>
       </c>
@@ -8608,8 +8691,17 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>50</v>
       </c>
@@ -8637,8 +8729,17 @@
       <c r="J10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>51</v>
       </c>
@@ -8666,8 +8767,17 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>52</v>
       </c>
@@ -8695,8 +8805,17 @@
       <c r="J12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>53</v>
       </c>
@@ -8724,8 +8843,17 @@
       <c r="J13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>54</v>
       </c>
@@ -8753,8 +8881,17 @@
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>55</v>
       </c>
@@ -8782,8 +8919,17 @@
       <c r="J15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>56</v>
       </c>
@@ -8811,8 +8957,17 @@
       <c r="J16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>57</v>
       </c>
@@ -8840,8 +8995,17 @@
       <c r="J17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>58</v>
       </c>
@@ -8869,8 +9033,17 @@
       <c r="J18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>59</v>
       </c>
@@ -8898,8 +9071,17 @@
       <c r="J19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>60</v>
       </c>
@@ -8927,8 +9109,17 @@
       <c r="J20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>61</v>
       </c>
@@ -8956,8 +9147,17 @@
       <c r="J21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>62</v>
       </c>
@@ -8985,8 +9185,17 @@
       <c r="J22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>63</v>
       </c>
@@ -9014,8 +9223,17 @@
       <c r="J23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>64</v>
       </c>
@@ -9043,8 +9261,17 @@
       <c r="J24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>65</v>
       </c>
@@ -9072,8 +9299,17 @@
       <c r="J25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>66</v>
       </c>
@@ -9101,8 +9337,17 @@
       <c r="J26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>67</v>
       </c>
@@ -9130,8 +9375,17 @@
       <c r="J27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>68</v>
       </c>
@@ -9158,6 +9412,15 @@
       </c>
       <c r="J28">
         <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) Added ESS data to 'Manchester_distribution_network_Kearsley' (and '29_bus_GB_transmission_network_with_Kearsley_GSP_group') network preset in network_factory.py
2) Update the demand profiles from scaling a single normalised profile to directly reading bus-specific demand profiles at DN level.
</commit_message>
<xml_diff>
--- a/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only_modified.xlsx
+++ b/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only_modified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\Manchester_Distribution_Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ABD00E-65D7-41CD-82B1-E382242383E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D841AA3-CE81-4627-BE26-A1C567AACBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_values" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="line&amp;trafo" sheetId="3" r:id="rId3"/>
     <sheet name="load" sheetId="4" r:id="rId4"/>
     <sheet name="gen" sheetId="5" r:id="rId5"/>
-    <sheet name="note" sheetId="6" r:id="rId6"/>
+    <sheet name="ess" sheetId="7" r:id="rId6"/>
+    <sheet name="note" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="156">
   <si>
     <t>Name</t>
   </si>
@@ -485,6 +486,27 @@
   </si>
   <si>
     <t>Gas Share</t>
+  </si>
+  <si>
+    <t>SOC_min</t>
+  </si>
+  <si>
+    <t>SOC_max</t>
+  </si>
+  <si>
+    <t>Pess_cap</t>
+  </si>
+  <si>
+    <t>Eess_cap</t>
+  </si>
+  <si>
+    <t>eff_ch</t>
+  </si>
+  <si>
+    <t>eff_dis</t>
+  </si>
+  <si>
+    <t>Due to data unavailability, it is assumed that the Energy Capacity (MWh) is 4 times the value of the Power Capacity (MW) for all ESS</t>
   </si>
 </sst>
 </file>
@@ -3477,7 +3499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
@@ -7032,7 +7054,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8341,8 +8363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9430,11 +9452,843 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F03022-DBB7-4796-A244-DA98EAB6A3C8}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="21.53125" customWidth="1"/>
+    <col min="3" max="3" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="10.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>0.19493845600000001</v>
+      </c>
+      <c r="E2">
+        <v>0.77975382400000004</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.95</v>
+      </c>
+      <c r="I2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>6.3732006190000003</v>
+      </c>
+      <c r="E3">
+        <v>25.492802476000001</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.95</v>
+      </c>
+      <c r="I3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>0.31130615</v>
+      </c>
+      <c r="E4">
+        <v>1.2452246</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.95</v>
+      </c>
+      <c r="I4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5">
+        <v>20.169742205999999</v>
+      </c>
+      <c r="E5">
+        <v>80.678968823999995</v>
+      </c>
+      <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.95</v>
+      </c>
+      <c r="I5">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6">
+        <v>6.0180641E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.240722564</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.95</v>
+      </c>
+      <c r="I6">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7">
+        <v>2.2602575999999999E-2</v>
+      </c>
+      <c r="E7">
+        <v>9.0410303999999997E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.95</v>
+      </c>
+      <c r="I7">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8">
+        <v>4.3687275999999997E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.17474910399999999</v>
+      </c>
+      <c r="F8">
+        <v>0.1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.95</v>
+      </c>
+      <c r="I8">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9">
+        <v>3.6711343E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.146845372</v>
+      </c>
+      <c r="F9">
+        <v>0.1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.95</v>
+      </c>
+      <c r="I9">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10">
+        <v>5.4359195999999999E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.21743678399999999</v>
+      </c>
+      <c r="F10">
+        <v>0.1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.95</v>
+      </c>
+      <c r="I10">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11">
+        <v>0.11587671400000001</v>
+      </c>
+      <c r="E11">
+        <v>0.46350685600000002</v>
+      </c>
+      <c r="F11">
+        <v>0.1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0.95</v>
+      </c>
+      <c r="I11">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12">
+        <v>7.1575979999999997E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.28630391999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.95</v>
+      </c>
+      <c r="I12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13">
+        <v>0.111187984</v>
+      </c>
+      <c r="E13">
+        <v>0.44475193600000001</v>
+      </c>
+      <c r="F13">
+        <v>0.1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0.95</v>
+      </c>
+      <c r="I13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14">
+        <v>5.2640237999999999E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.210560952</v>
+      </c>
+      <c r="F14">
+        <v>0.1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0.95</v>
+      </c>
+      <c r="I14">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15">
+        <v>2.1919702999999999E-2</v>
+      </c>
+      <c r="E15">
+        <v>8.7678811999999995E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0.95</v>
+      </c>
+      <c r="I15">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16">
+        <v>3.9309358000000003E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.15723743200000001</v>
+      </c>
+      <c r="F16">
+        <v>0.1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0.95</v>
+      </c>
+      <c r="I16">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17">
+        <v>1.0525646E-2</v>
+      </c>
+      <c r="E17">
+        <v>4.2102583999999998E-2</v>
+      </c>
+      <c r="F17">
+        <v>0.1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0.95</v>
+      </c>
+      <c r="I17">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18">
+        <v>4.2206566000000001E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.168826264</v>
+      </c>
+      <c r="F18">
+        <v>0.1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0.95</v>
+      </c>
+      <c r="I18">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19">
+        <v>5.0311228999999999E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.201244916</v>
+      </c>
+      <c r="F19">
+        <v>0.1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0.95</v>
+      </c>
+      <c r="I19">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20">
+        <v>4.0473565000000003E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.16189426000000001</v>
+      </c>
+      <c r="F20">
+        <v>0.1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0.95</v>
+      </c>
+      <c r="I20">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21">
+        <v>3.9270262E-2</v>
+      </c>
+      <c r="E21">
+        <v>0.157081048</v>
+      </c>
+      <c r="F21">
+        <v>0.1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0.95</v>
+      </c>
+      <c r="I21">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
+        <v>3.9695978999999999E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.158783916</v>
+      </c>
+      <c r="F22">
+        <v>0.1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0.95</v>
+      </c>
+      <c r="I22">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23">
+        <v>4.9513544999999999E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.19805418</v>
+      </c>
+      <c r="F23">
+        <v>0.1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0.95</v>
+      </c>
+      <c r="I23">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24">
+        <v>2.6664064000000001E-2</v>
+      </c>
+      <c r="E24">
+        <v>0.106656256</v>
+      </c>
+      <c r="F24">
+        <v>0.1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0.95</v>
+      </c>
+      <c r="I24">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25">
+        <v>1.4266869E-2</v>
+      </c>
+      <c r="E25">
+        <v>5.7067475999999999E-2</v>
+      </c>
+      <c r="F25">
+        <v>0.1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0.95</v>
+      </c>
+      <c r="I25">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26">
+        <v>1.0840102000000001E-2</v>
+      </c>
+      <c r="E26">
+        <v>4.3360408000000003E-2</v>
+      </c>
+      <c r="F26">
+        <v>0.1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0.95</v>
+      </c>
+      <c r="I26">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27">
+        <v>3.7917307999999997E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.15166923199999999</v>
+      </c>
+      <c r="F27">
+        <v>0.1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0.95</v>
+      </c>
+      <c r="I27">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28">
+        <v>3.7005827999999998E-2</v>
+      </c>
+      <c r="E28">
+        <v>0.14802331199999999</v>
+      </c>
+      <c r="F28">
+        <v>0.1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0.95</v>
+      </c>
+      <c r="I28">
+        <v>0.95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1A0D1A-F6F3-4395-9C5A-D200374D67D4}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9458,6 +10312,14 @@
         <v>142</v>
       </c>
     </row>
+    <row r="3" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1) Updated the structure of the part 'elif name == '29_bus_GB_transmission_network_with_Kearsley_GSP_group':' in network_factory.py.
2) Small fixes across network_factory.py.
</commit_message>
<xml_diff>
--- a/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only_modified.xlsx
+++ b/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only_modified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\Manchester_Distribution_Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D841AA3-CE81-4627-BE26-A1C567AACBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A174BEC3-BBA7-42E7-A424-00F5342EDD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_values" sheetId="1" r:id="rId1"/>
@@ -437,15 +437,9 @@
     <t>Qg_min</t>
   </si>
   <si>
-    <t>gen_cost_coef_1</t>
-  </si>
-  <si>
     <t>Type (1 for line, 0 for transformer)</t>
   </si>
   <si>
-    <t>gen_cost_coef_0</t>
-  </si>
-  <si>
     <t>S_max (MW)</t>
   </si>
   <si>
@@ -507,6 +501,12 @@
   </si>
   <si>
     <t>Due to data unavailability, it is assumed that the Energy Capacity (MWh) is 4 times the value of the Power Capacity (MW) for all ESS</t>
+  </si>
+  <si>
+    <t>gen_cost_coef_0 (Gas)</t>
+  </si>
+  <si>
+    <t>gen_cost_coef_1 (Gas)</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
   <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -933,10 +933,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>11</v>
@@ -3536,10 +3536,10 @@
         <v>91</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>92</v>
@@ -3554,10 +3554,10 @@
         <v>95</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
@@ -7101,13 +7101,13 @@
         <v>103</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
@@ -8363,8 +8363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8373,7 +8373,7 @@
     <col min="3" max="3" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="10.59765625" customWidth="1"/>
-    <col min="9" max="10" width="15.59765625" customWidth="1"/>
+    <col min="9" max="10" width="19.3984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.19921875" customWidth="1"/>
   </cols>
@@ -8404,19 +8404,19 @@
         <v>131</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
@@ -8445,7 +8445,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -8483,7 +8483,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -8521,7 +8521,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -8559,7 +8559,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -8597,7 +8597,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -8635,7 +8635,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -8673,7 +8673,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -8711,7 +8711,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -8749,7 +8749,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -8787,7 +8787,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -8825,7 +8825,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -8863,7 +8863,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -8901,7 +8901,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -8939,7 +8939,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -8977,7 +8977,7 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -9015,7 +9015,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -9053,7 +9053,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -9091,7 +9091,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -9129,7 +9129,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -9167,7 +9167,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -9205,7 +9205,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -9243,7 +9243,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -9281,7 +9281,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -9319,7 +9319,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -9357,7 +9357,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -9395,7 +9395,7 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -9433,7 +9433,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -9455,7 +9455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F03022-DBB7-4796-A244-DA98EAB6A3C8}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -9477,22 +9477,22 @@
         <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
@@ -10298,10 +10298,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
@@ -10309,7 +10309,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
@@ -10317,7 +10317,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) In network.py, added methods 'solve_combined_opf_in_chunks' (which allows to split an opf with a large number of timesteps into multiple chunks and solve separately) and '_analyze_load_shedding' (which checks for any load shedding values in the opf results (either from a single run or from a set of chunks)).
2) Modified 'Kearsley_GSP_group_only_modified.xlsx' to ensure there's no load shedding in the normal-operation scenario.

3) Modified visualize_network_topology.py to improve the clarity of labels.
</commit_message>
<xml_diff>
--- a/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only_modified.xlsx
+++ b/Input_Data/Manchester_Distribution_Network/Kearsley_GSP_group_only_modified.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\Manchester_Distribution_Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A174BEC3-BBA7-42E7-A424-00F5342EDD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7AEFB6-499C-493C-B10D-012E2449BA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3499,8 +3499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7054,7 +7054,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A16" sqref="A16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8364,7 +8364,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8430,7 +8430,7 @@
         <v>27</v>
       </c>
       <c r="E2">
-        <v>3.5625888020000001</v>
+        <v>23.562588802</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -8468,7 +8468,7 @@
         <v>34</v>
       </c>
       <c r="E3">
-        <v>15.716287454</v>
+        <v>25.716287454</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8506,7 +8506,7 @@
         <v>42</v>
       </c>
       <c r="E4">
-        <v>11.635689107999999</v>
+        <v>24.635689108000001</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -8582,7 +8582,7 @@
         <v>104</v>
       </c>
       <c r="E6">
-        <v>0.589363521</v>
+        <v>10.589363520999999</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -8658,7 +8658,7 @@
         <v>106</v>
       </c>
       <c r="E8">
-        <v>0.80344782900000011</v>
+        <v>2.803447829</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -8810,7 +8810,7 @@
         <v>110</v>
       </c>
       <c r="E12">
-        <v>5.3985405980000003</v>
+        <v>6.3985405980000003</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -8848,7 +8848,7 @@
         <v>111</v>
       </c>
       <c r="E13">
-        <v>4.0841158010000003</v>
+        <v>11.084115800999999</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -8962,7 +8962,7 @@
         <v>114</v>
       </c>
       <c r="E16">
-        <v>0.78897617400000009</v>
+        <v>7.8889761739999997</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -9038,7 +9038,7 @@
         <v>116</v>
       </c>
       <c r="E18">
-        <v>1.2779157539999999</v>
+        <v>4.2779157540000003</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -9380,7 +9380,7 @@
         <v>125</v>
       </c>
       <c r="E27">
-        <v>1.116071569</v>
+        <v>4.4160715689999996</v>
       </c>
       <c r="F27">
         <v>0</v>

</xml_diff>